<commit_message>
Mise en ligne gestion de projet.
</commit_message>
<xml_diff>
--- a/Gestion/Burndown.xlsx
+++ b/Gestion/Burndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Projet S2\github\Gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projetS2\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -402,6 +402,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -411,15 +420,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,7 +559,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>145</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>130</c:v>
@@ -1650,7 +1650,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1660,13 +1660,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1705,12 +1705,12 @@
         <v>141</v>
       </c>
       <c r="D4" s="1">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4">
         <f t="shared" ref="F4:F11" si="0">D4-C4</f>
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="M4" s="1"/>
     </row>
@@ -1806,7 +1806,7 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="32" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="6">
@@ -1827,7 +1827,7 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1">
@@ -1848,7 +1848,7 @@
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="1">
@@ -1889,13 +1889,13 @@
       <c r="B13" s="1"/>
       <c r="C13" s="6"/>
       <c r="D13" s="1"/>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="35"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="40"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -2044,7 +2044,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="24">
@@ -2059,13 +2059,13 @@
       <c r="K20" s="24">
         <v>4</v>
       </c>
-      <c r="L20" s="38">
+      <c r="L20" s="33">
         <v>4</v>
       </c>
       <c r="M20" s="4"/>
     </row>
     <row r="21" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="31" t="s">
         <v>20</v>
       </c>
       <c r="H21" s="17">
@@ -2080,13 +2080,13 @@
       <c r="K21" s="17">
         <v>4</v>
       </c>
-      <c r="L21" s="39">
+      <c r="L21" s="34">
         <v>4</v>
       </c>
       <c r="M21" s="4"/>
     </row>
     <row r="22" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G22" s="40" t="s">
+      <c r="G22" s="35" t="s">
         <v>21</v>
       </c>
       <c r="H22" s="19">
@@ -2181,18 +2181,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2328,14 +2328,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97EC856-B55B-4E4D-BE05-EBDC7337E598}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F526679E-0FD3-4499-8752-D553AA35AF2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2347,6 +2339,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="de03dccb-4976-458f-8f7d-dd981b9011ac"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97EC856-B55B-4E4D-BE05-EBDC7337E598}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>